<commit_message>
Phát thảo kiến trúc hệ thống theo góc nhìn của Khách hàng.
</commit_message>
<xml_diff>
--- a/doc/requirement/GW_User requirement document.xlsx
+++ b/doc/requirement/GW_User requirement document.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BigBusiness\TimLoTrinhGiaoHang\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProjects\github.com\mksgroup\goodway\git\goodway\doc\requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="15480" windowHeight="8130" tabRatio="705" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="15480" windowHeight="8130" tabRatio="705" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Record of change" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -213,6 +213,24 @@
   </si>
   <si>
     <t>[Kiến trúc hệ thống với góc nhìn của người dùng - Các công ty vận chuyển]</t>
+  </si>
+  <si>
+    <t>Server side</t>
+  </si>
+  <si>
+    <t>Client side</t>
+  </si>
+  <si>
+    <t>User service: cung cấp các dịch vụ đăng nhập, cấp phát tài khoản người dùng</t>
+  </si>
+  <si>
+    <t>Delivery Plan service cung cấp dịch vụ lập kế hoạch giao hàng tối ưu.</t>
+  </si>
+  <si>
+    <t>Find Path service: cung cấp dịch vụ lập lộ trình giao hàng tối ưu.</t>
+  </si>
+  <si>
+    <t>Reporting service: cung cấp dịch vụ theo dõi tiến độ giao hàng, báo cáo số liệu</t>
   </si>
 </sst>
 </file>
@@ -488,7 +506,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="26">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -636,6 +654,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1114,7 +1138,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="23" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="20" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1274,138 +1298,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="36" fillId="0" borderId="0" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="36" fillId="0" borderId="13" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="25" fillId="0" borderId="35" xfId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="25" fillId="0" borderId="36" xfId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="28" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="30" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="14" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="15" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="32" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="19" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="20" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="21" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="16" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="17" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="18" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="28" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="30" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="14" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="15" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="31" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="32" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="23" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="34" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="32" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="23" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="36" fillId="0" borderId="0" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="34" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1420,6 +1312,144 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="28" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="30" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="14" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="15" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="32" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="19" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="20" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="21" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="16" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="17" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="18" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="28" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="30" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="14" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="15" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="31" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="32" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="23" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="34" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="32" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="23" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="25" fillId="0" borderId="35" xfId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="25" fillId="0" borderId="36" xfId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="36" fillId="0" borderId="0" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="36" fillId="0" borderId="13" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1513,6 +1543,786 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>5195</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>31173</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>86591</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>60614</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2862695" y="1581150"/>
+          <a:ext cx="81396" cy="4029941"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>69272</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>51955</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>164522</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>121228</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1368136" y="1601932"/>
+          <a:ext cx="874568" cy="1402773"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Web Browser</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>51954</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>129887</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>187036</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>91787</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Snip Single Corner Rectangle 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1350818" y="3203864"/>
+          <a:ext cx="914400" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip1Rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Smart phone</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>51954</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>8660</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>187036</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>161060</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Snip Single Corner Rectangle 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1350818" y="4416137"/>
+          <a:ext cx="914400" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip1Rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Tablet</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>187036</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>103909</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>22513</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161060</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3564081" y="1844386"/>
+          <a:ext cx="874568" cy="2343151"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Server</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Gateway</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>71003</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>157596</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>242454</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>164523</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5526230" y="1898073"/>
+          <a:ext cx="3028951" cy="768927"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Google Map</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>71004</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>166255</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>233796</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>164523</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5526231" y="3049732"/>
+          <a:ext cx="3020292" cy="1141268"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Microservices</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>34636</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>164524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>259495</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Up-Down Arrow 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6788727" y="2667001"/>
+          <a:ext cx="484632" cy="389658"/>
+        </a:xfrm>
+        <a:prstGeom prst="upDownArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+            <a:gd name="adj2" fmla="val 32133"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>216478</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>138546</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>17318</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>86591</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rounded Rectangle 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5671705" y="3403023"/>
+          <a:ext cx="1359477" cy="329045"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>User service</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>91787</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>135082</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>83127</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rounded Rectangle 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7105651" y="3399559"/>
+          <a:ext cx="1359477" cy="329045"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Delivery Plan service</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>213014</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>13854</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>109105</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rounded Rectangle 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5668241" y="3806537"/>
+          <a:ext cx="1359477" cy="329045"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Reporting service</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>88323</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>157596</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>148937</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>105641</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rounded Rectangle 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7102187" y="3803073"/>
+          <a:ext cx="1359477" cy="329045"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Find</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Path service</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>17318</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>181841</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Left-Right Arrow 13"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4675909" y="3472295"/>
+          <a:ext cx="710046" cy="355023"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftRightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>259772</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>143741</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171034</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Cloud Callout 14"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2337954" y="2502477"/>
+          <a:ext cx="1182832" cy="933034"/>
+        </a:xfrm>
+        <a:prstGeom prst="cloudCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -12780"/>
+            <a:gd name="adj2" fmla="val 53219"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Internet</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2072,138 +2882,138 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="81" t="s">
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="83"/>
-      <c r="W1" s="87" t="s">
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="80"/>
+      <c r="P1" s="80"/>
+      <c r="Q1" s="80"/>
+      <c r="R1" s="80"/>
+      <c r="S1" s="80"/>
+      <c r="T1" s="80"/>
+      <c r="U1" s="80"/>
+      <c r="V1" s="81"/>
+      <c r="W1" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="88"/>
-      <c r="Y1" s="88"/>
-      <c r="Z1" s="88"/>
-      <c r="AA1" s="88"/>
-      <c r="AB1" s="88"/>
-      <c r="AC1" s="88"/>
-      <c r="AD1" s="88"/>
-      <c r="AE1" s="88"/>
-      <c r="AF1" s="88"/>
-      <c r="AG1" s="88"/>
-      <c r="AH1" s="88"/>
-      <c r="AI1" s="88"/>
-      <c r="AJ1" s="89"/>
+      <c r="X1" s="86"/>
+      <c r="Y1" s="86"/>
+      <c r="Z1" s="86"/>
+      <c r="AA1" s="86"/>
+      <c r="AB1" s="86"/>
+      <c r="AC1" s="86"/>
+      <c r="AD1" s="86"/>
+      <c r="AE1" s="86"/>
+      <c r="AF1" s="86"/>
+      <c r="AG1" s="86"/>
+      <c r="AH1" s="86"/>
+      <c r="AI1" s="86"/>
+      <c r="AJ1" s="87"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="79"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
-      <c r="R2" s="85"/>
-      <c r="S2" s="85"/>
-      <c r="T2" s="85"/>
-      <c r="U2" s="85"/>
-      <c r="V2" s="86"/>
-      <c r="W2" s="90" t="s">
+      <c r="A2" s="77"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
+      <c r="S2" s="83"/>
+      <c r="T2" s="83"/>
+      <c r="U2" s="83"/>
+      <c r="V2" s="84"/>
+      <c r="W2" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="X2" s="91"/>
-      <c r="Y2" s="91"/>
-      <c r="Z2" s="91"/>
-      <c r="AA2" s="91"/>
-      <c r="AB2" s="91"/>
-      <c r="AC2" s="91"/>
-      <c r="AD2" s="91"/>
-      <c r="AE2" s="91"/>
-      <c r="AF2" s="91"/>
-      <c r="AG2" s="91"/>
-      <c r="AH2" s="91"/>
-      <c r="AI2" s="91"/>
-      <c r="AJ2" s="92"/>
+      <c r="X2" s="89"/>
+      <c r="Y2" s="89"/>
+      <c r="Z2" s="89"/>
+      <c r="AA2" s="89"/>
+      <c r="AB2" s="89"/>
+      <c r="AC2" s="89"/>
+      <c r="AD2" s="89"/>
+      <c r="AE2" s="89"/>
+      <c r="AF2" s="89"/>
+      <c r="AG2" s="89"/>
+      <c r="AH2" s="89"/>
+      <c r="AI2" s="89"/>
+      <c r="AJ2" s="90"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="94"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="97" t="s">
+      <c r="B3" s="92"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="94" t="s">
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="94"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="103"/>
-      <c r="M3" s="105" t="s">
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
-      <c r="Q3" s="98"/>
-      <c r="R3" s="98"/>
-      <c r="S3" s="98"/>
-      <c r="T3" s="98"/>
-      <c r="U3" s="98"/>
-      <c r="V3" s="106"/>
+      <c r="N3" s="96"/>
+      <c r="O3" s="96"/>
+      <c r="P3" s="96"/>
+      <c r="Q3" s="96"/>
+      <c r="R3" s="96"/>
+      <c r="S3" s="96"/>
+      <c r="T3" s="96"/>
+      <c r="U3" s="96"/>
+      <c r="V3" s="104"/>
       <c r="W3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
-      <c r="Z3" s="72">
+      <c r="Z3" s="107">
         <v>43205</v>
       </c>
-      <c r="AA3" s="72"/>
-      <c r="AB3" s="72"/>
-      <c r="AC3" s="73"/>
+      <c r="AA3" s="107"/>
+      <c r="AB3" s="107"/>
+      <c r="AC3" s="108"/>
       <c r="AD3" s="3" t="s">
         <v>9</v>
       </c>
@@ -2215,46 +3025,46 @@
       <c r="AJ3" s="111"/>
     </row>
     <row r="4" spans="1:36" ht="15" customHeight="1">
-      <c r="A4" s="95"/>
-      <c r="B4" s="96"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="104"/>
-      <c r="M4" s="107"/>
-      <c r="N4" s="101"/>
-      <c r="O4" s="101"/>
-      <c r="P4" s="101"/>
-      <c r="Q4" s="101"/>
-      <c r="R4" s="101"/>
-      <c r="S4" s="101"/>
-      <c r="T4" s="101"/>
-      <c r="U4" s="101"/>
-      <c r="V4" s="108"/>
+      <c r="A4" s="93"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="94"/>
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
+      <c r="L4" s="102"/>
+      <c r="M4" s="105"/>
+      <c r="N4" s="99"/>
+      <c r="O4" s="99"/>
+      <c r="P4" s="99"/>
+      <c r="Q4" s="99"/>
+      <c r="R4" s="99"/>
+      <c r="S4" s="99"/>
+      <c r="T4" s="99"/>
+      <c r="U4" s="99"/>
+      <c r="V4" s="106"/>
       <c r="W4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
-      <c r="Z4" s="72"/>
-      <c r="AA4" s="72"/>
-      <c r="AB4" s="72"/>
-      <c r="AC4" s="73"/>
+      <c r="Z4" s="107"/>
+      <c r="AA4" s="107"/>
+      <c r="AB4" s="107"/>
+      <c r="AC4" s="108"/>
       <c r="AD4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AE4" s="7"/>
       <c r="AF4" s="8"/>
-      <c r="AG4" s="74"/>
-      <c r="AH4" s="75"/>
-      <c r="AI4" s="75"/>
-      <c r="AJ4" s="76"/>
+      <c r="AG4" s="114"/>
+      <c r="AH4" s="115"/>
+      <c r="AI4" s="115"/>
+      <c r="AJ4" s="116"/>
     </row>
     <row r="5" spans="1:36" ht="15.75">
       <c r="A5" s="35">
@@ -2991,81 +3801,81 @@
       <c r="A23" s="43"/>
       <c r="B23" s="39"/>
       <c r="C23" s="39"/>
-      <c r="D23" s="112" t="s">
+      <c r="D23" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="68" t="s">
+      <c r="E23" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="68"/>
-      <c r="L23" s="68"/>
-      <c r="M23" s="68"/>
-      <c r="N23" s="68"/>
-      <c r="O23" s="68"/>
-      <c r="P23" s="68"/>
-      <c r="Q23" s="68"/>
-      <c r="R23" s="68"/>
-      <c r="S23" s="68"/>
-      <c r="T23" s="68"/>
-      <c r="U23" s="68"/>
-      <c r="V23" s="68"/>
-      <c r="W23" s="68"/>
-      <c r="X23" s="68"/>
-      <c r="Y23" s="68"/>
-      <c r="Z23" s="68"/>
-      <c r="AA23" s="68"/>
-      <c r="AB23" s="68"/>
-      <c r="AC23" s="68"/>
-      <c r="AD23" s="68"/>
-      <c r="AE23" s="68"/>
-      <c r="AF23" s="68"/>
-      <c r="AG23" s="68"/>
-      <c r="AH23" s="68"/>
-      <c r="AI23" s="68"/>
-      <c r="AJ23" s="69"/>
+      <c r="F23" s="117"/>
+      <c r="G23" s="117"/>
+      <c r="H23" s="117"/>
+      <c r="I23" s="117"/>
+      <c r="J23" s="117"/>
+      <c r="K23" s="117"/>
+      <c r="L23" s="117"/>
+      <c r="M23" s="117"/>
+      <c r="N23" s="117"/>
+      <c r="O23" s="117"/>
+      <c r="P23" s="117"/>
+      <c r="Q23" s="117"/>
+      <c r="R23" s="117"/>
+      <c r="S23" s="117"/>
+      <c r="T23" s="117"/>
+      <c r="U23" s="117"/>
+      <c r="V23" s="117"/>
+      <c r="W23" s="117"/>
+      <c r="X23" s="117"/>
+      <c r="Y23" s="117"/>
+      <c r="Z23" s="117"/>
+      <c r="AA23" s="117"/>
+      <c r="AB23" s="117"/>
+      <c r="AC23" s="117"/>
+      <c r="AD23" s="117"/>
+      <c r="AE23" s="117"/>
+      <c r="AF23" s="117"/>
+      <c r="AG23" s="117"/>
+      <c r="AH23" s="117"/>
+      <c r="AI23" s="117"/>
+      <c r="AJ23" s="118"/>
     </row>
     <row r="24" spans="1:36" ht="15.75" customHeight="1">
       <c r="A24" s="43"/>
       <c r="B24" s="39"/>
       <c r="C24" s="39"/>
-      <c r="D24" s="112"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="68"/>
-      <c r="I24" s="68"/>
-      <c r="J24" s="68"/>
-      <c r="K24" s="68"/>
-      <c r="L24" s="68"/>
-      <c r="M24" s="68"/>
-      <c r="N24" s="68"/>
-      <c r="O24" s="68"/>
-      <c r="P24" s="68"/>
-      <c r="Q24" s="68"/>
-      <c r="R24" s="68"/>
-      <c r="S24" s="68"/>
-      <c r="T24" s="68"/>
-      <c r="U24" s="68"/>
-      <c r="V24" s="68"/>
-      <c r="W24" s="68"/>
-      <c r="X24" s="68"/>
-      <c r="Y24" s="68"/>
-      <c r="Z24" s="68"/>
-      <c r="AA24" s="68"/>
-      <c r="AB24" s="68"/>
-      <c r="AC24" s="68"/>
-      <c r="AD24" s="68"/>
-      <c r="AE24" s="68"/>
-      <c r="AF24" s="68"/>
-      <c r="AG24" s="68"/>
-      <c r="AH24" s="68"/>
-      <c r="AI24" s="68"/>
-      <c r="AJ24" s="69"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="117"/>
+      <c r="F24" s="117"/>
+      <c r="G24" s="117"/>
+      <c r="H24" s="117"/>
+      <c r="I24" s="117"/>
+      <c r="J24" s="117"/>
+      <c r="K24" s="117"/>
+      <c r="L24" s="117"/>
+      <c r="M24" s="117"/>
+      <c r="N24" s="117"/>
+      <c r="O24" s="117"/>
+      <c r="P24" s="117"/>
+      <c r="Q24" s="117"/>
+      <c r="R24" s="117"/>
+      <c r="S24" s="117"/>
+      <c r="T24" s="117"/>
+      <c r="U24" s="117"/>
+      <c r="V24" s="117"/>
+      <c r="W24" s="117"/>
+      <c r="X24" s="117"/>
+      <c r="Y24" s="117"/>
+      <c r="Z24" s="117"/>
+      <c r="AA24" s="117"/>
+      <c r="AB24" s="117"/>
+      <c r="AC24" s="117"/>
+      <c r="AD24" s="117"/>
+      <c r="AE24" s="117"/>
+      <c r="AF24" s="117"/>
+      <c r="AG24" s="117"/>
+      <c r="AH24" s="117"/>
+      <c r="AI24" s="117"/>
+      <c r="AJ24" s="118"/>
     </row>
     <row r="25" spans="1:36" ht="15.75" customHeight="1">
       <c r="A25" s="43"/>
@@ -3148,7 +3958,7 @@
       <c r="AJ26" s="37"/>
     </row>
     <row r="27" spans="1:36" ht="15.75">
-      <c r="A27" s="113"/>
+      <c r="A27" s="69"/>
       <c r="B27" s="38"/>
       <c r="C27" s="38"/>
       <c r="D27" s="38"/>
@@ -3232,164 +4042,169 @@
       <c r="B29" s="67">
         <v>2</v>
       </c>
-      <c r="C29" s="70" t="s">
+      <c r="C29" s="112" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="70"/>
-      <c r="E29" s="70"/>
-      <c r="F29" s="70"/>
-      <c r="G29" s="70"/>
-      <c r="H29" s="70"/>
-      <c r="I29" s="70"/>
-      <c r="J29" s="70"/>
-      <c r="K29" s="70"/>
-      <c r="L29" s="70"/>
-      <c r="M29" s="70"/>
-      <c r="N29" s="70"/>
-      <c r="O29" s="70"/>
-      <c r="P29" s="70"/>
-      <c r="Q29" s="70"/>
-      <c r="R29" s="70"/>
-      <c r="S29" s="70"/>
-      <c r="T29" s="70"/>
-      <c r="U29" s="70"/>
-      <c r="V29" s="70"/>
-      <c r="W29" s="70"/>
-      <c r="X29" s="70"/>
-      <c r="Y29" s="70"/>
-      <c r="Z29" s="70"/>
-      <c r="AA29" s="70"/>
-      <c r="AB29" s="70"/>
-      <c r="AC29" s="70"/>
-      <c r="AD29" s="70"/>
-      <c r="AE29" s="70"/>
-      <c r="AF29" s="70"/>
-      <c r="AG29" s="70"/>
-      <c r="AH29" s="70"/>
-      <c r="AI29" s="70"/>
-      <c r="AJ29" s="71"/>
+      <c r="D29" s="112"/>
+      <c r="E29" s="112"/>
+      <c r="F29" s="112"/>
+      <c r="G29" s="112"/>
+      <c r="H29" s="112"/>
+      <c r="I29" s="112"/>
+      <c r="J29" s="112"/>
+      <c r="K29" s="112"/>
+      <c r="L29" s="112"/>
+      <c r="M29" s="112"/>
+      <c r="N29" s="112"/>
+      <c r="O29" s="112"/>
+      <c r="P29" s="112"/>
+      <c r="Q29" s="112"/>
+      <c r="R29" s="112"/>
+      <c r="S29" s="112"/>
+      <c r="T29" s="112"/>
+      <c r="U29" s="112"/>
+      <c r="V29" s="112"/>
+      <c r="W29" s="112"/>
+      <c r="X29" s="112"/>
+      <c r="Y29" s="112"/>
+      <c r="Z29" s="112"/>
+      <c r="AA29" s="112"/>
+      <c r="AB29" s="112"/>
+      <c r="AC29" s="112"/>
+      <c r="AD29" s="112"/>
+      <c r="AE29" s="112"/>
+      <c r="AF29" s="112"/>
+      <c r="AG29" s="112"/>
+      <c r="AH29" s="112"/>
+      <c r="AI29" s="112"/>
+      <c r="AJ29" s="113"/>
     </row>
     <row r="30" spans="1:36" ht="15.75">
       <c r="A30" s="43"/>
       <c r="B30" s="38"/>
-      <c r="C30" s="70"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="70"/>
-      <c r="F30" s="70"/>
-      <c r="G30" s="70"/>
-      <c r="H30" s="70"/>
-      <c r="I30" s="70"/>
-      <c r="J30" s="70"/>
-      <c r="K30" s="70"/>
-      <c r="L30" s="70"/>
-      <c r="M30" s="70"/>
-      <c r="N30" s="70"/>
-      <c r="O30" s="70"/>
-      <c r="P30" s="70"/>
-      <c r="Q30" s="70"/>
-      <c r="R30" s="70"/>
-      <c r="S30" s="70"/>
-      <c r="T30" s="70"/>
-      <c r="U30" s="70"/>
-      <c r="V30" s="70"/>
-      <c r="W30" s="70"/>
-      <c r="X30" s="70"/>
-      <c r="Y30" s="70"/>
-      <c r="Z30" s="70"/>
-      <c r="AA30" s="70"/>
-      <c r="AB30" s="70"/>
-      <c r="AC30" s="70"/>
-      <c r="AD30" s="70"/>
-      <c r="AE30" s="70"/>
-      <c r="AF30" s="70"/>
-      <c r="AG30" s="70"/>
-      <c r="AH30" s="70"/>
-      <c r="AI30" s="70"/>
-      <c r="AJ30" s="71"/>
+      <c r="C30" s="112"/>
+      <c r="D30" s="112"/>
+      <c r="E30" s="112"/>
+      <c r="F30" s="112"/>
+      <c r="G30" s="112"/>
+      <c r="H30" s="112"/>
+      <c r="I30" s="112"/>
+      <c r="J30" s="112"/>
+      <c r="K30" s="112"/>
+      <c r="L30" s="112"/>
+      <c r="M30" s="112"/>
+      <c r="N30" s="112"/>
+      <c r="O30" s="112"/>
+      <c r="P30" s="112"/>
+      <c r="Q30" s="112"/>
+      <c r="R30" s="112"/>
+      <c r="S30" s="112"/>
+      <c r="T30" s="112"/>
+      <c r="U30" s="112"/>
+      <c r="V30" s="112"/>
+      <c r="W30" s="112"/>
+      <c r="X30" s="112"/>
+      <c r="Y30" s="112"/>
+      <c r="Z30" s="112"/>
+      <c r="AA30" s="112"/>
+      <c r="AB30" s="112"/>
+      <c r="AC30" s="112"/>
+      <c r="AD30" s="112"/>
+      <c r="AE30" s="112"/>
+      <c r="AF30" s="112"/>
+      <c r="AG30" s="112"/>
+      <c r="AH30" s="112"/>
+      <c r="AI30" s="112"/>
+      <c r="AJ30" s="113"/>
     </row>
     <row r="31" spans="1:36" ht="15.75">
       <c r="A31" s="43"/>
       <c r="B31" s="67">
         <v>3</v>
       </c>
-      <c r="C31" s="70" t="s">
+      <c r="C31" s="112" t="s">
         <v>40</v>
       </c>
-      <c r="D31" s="70"/>
-      <c r="E31" s="70"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="70"/>
-      <c r="H31" s="70"/>
-      <c r="I31" s="70"/>
-      <c r="J31" s="70"/>
-      <c r="K31" s="70"/>
-      <c r="L31" s="70"/>
-      <c r="M31" s="70"/>
-      <c r="N31" s="70"/>
-      <c r="O31" s="70"/>
-      <c r="P31" s="70"/>
-      <c r="Q31" s="70"/>
-      <c r="R31" s="70"/>
-      <c r="S31" s="70"/>
-      <c r="T31" s="70"/>
-      <c r="U31" s="70"/>
-      <c r="V31" s="70"/>
-      <c r="W31" s="70"/>
-      <c r="X31" s="70"/>
-      <c r="Y31" s="70"/>
-      <c r="Z31" s="70"/>
-      <c r="AA31" s="70"/>
-      <c r="AB31" s="70"/>
-      <c r="AC31" s="70"/>
-      <c r="AD31" s="70"/>
-      <c r="AE31" s="70"/>
-      <c r="AF31" s="70"/>
-      <c r="AG31" s="70"/>
-      <c r="AH31" s="70"/>
-      <c r="AI31" s="70"/>
-      <c r="AJ31" s="71"/>
+      <c r="D31" s="112"/>
+      <c r="E31" s="112"/>
+      <c r="F31" s="112"/>
+      <c r="G31" s="112"/>
+      <c r="H31" s="112"/>
+      <c r="I31" s="112"/>
+      <c r="J31" s="112"/>
+      <c r="K31" s="112"/>
+      <c r="L31" s="112"/>
+      <c r="M31" s="112"/>
+      <c r="N31" s="112"/>
+      <c r="O31" s="112"/>
+      <c r="P31" s="112"/>
+      <c r="Q31" s="112"/>
+      <c r="R31" s="112"/>
+      <c r="S31" s="112"/>
+      <c r="T31" s="112"/>
+      <c r="U31" s="112"/>
+      <c r="V31" s="112"/>
+      <c r="W31" s="112"/>
+      <c r="X31" s="112"/>
+      <c r="Y31" s="112"/>
+      <c r="Z31" s="112"/>
+      <c r="AA31" s="112"/>
+      <c r="AB31" s="112"/>
+      <c r="AC31" s="112"/>
+      <c r="AD31" s="112"/>
+      <c r="AE31" s="112"/>
+      <c r="AF31" s="112"/>
+      <c r="AG31" s="112"/>
+      <c r="AH31" s="112"/>
+      <c r="AI31" s="112"/>
+      <c r="AJ31" s="113"/>
     </row>
     <row r="32" spans="1:36" ht="15.75">
       <c r="A32" s="53"/>
       <c r="B32" s="54"/>
-      <c r="C32" s="70"/>
-      <c r="D32" s="70"/>
-      <c r="E32" s="70"/>
-      <c r="F32" s="70"/>
-      <c r="G32" s="70"/>
-      <c r="H32" s="70"/>
-      <c r="I32" s="70"/>
-      <c r="J32" s="70"/>
-      <c r="K32" s="70"/>
-      <c r="L32" s="70"/>
-      <c r="M32" s="70"/>
-      <c r="N32" s="70"/>
-      <c r="O32" s="70"/>
-      <c r="P32" s="70"/>
-      <c r="Q32" s="70"/>
-      <c r="R32" s="70"/>
-      <c r="S32" s="70"/>
-      <c r="T32" s="70"/>
-      <c r="U32" s="70"/>
-      <c r="V32" s="70"/>
-      <c r="W32" s="70"/>
-      <c r="X32" s="70"/>
-      <c r="Y32" s="70"/>
-      <c r="Z32" s="70"/>
-      <c r="AA32" s="70"/>
-      <c r="AB32" s="70"/>
-      <c r="AC32" s="70"/>
-      <c r="AD32" s="70"/>
-      <c r="AE32" s="70"/>
-      <c r="AF32" s="70"/>
-      <c r="AG32" s="70"/>
-      <c r="AH32" s="70"/>
-      <c r="AI32" s="70"/>
-      <c r="AJ32" s="71"/>
+      <c r="C32" s="112"/>
+      <c r="D32" s="112"/>
+      <c r="E32" s="112"/>
+      <c r="F32" s="112"/>
+      <c r="G32" s="112"/>
+      <c r="H32" s="112"/>
+      <c r="I32" s="112"/>
+      <c r="J32" s="112"/>
+      <c r="K32" s="112"/>
+      <c r="L32" s="112"/>
+      <c r="M32" s="112"/>
+      <c r="N32" s="112"/>
+      <c r="O32" s="112"/>
+      <c r="P32" s="112"/>
+      <c r="Q32" s="112"/>
+      <c r="R32" s="112"/>
+      <c r="S32" s="112"/>
+      <c r="T32" s="112"/>
+      <c r="U32" s="112"/>
+      <c r="V32" s="112"/>
+      <c r="W32" s="112"/>
+      <c r="X32" s="112"/>
+      <c r="Y32" s="112"/>
+      <c r="Z32" s="112"/>
+      <c r="AA32" s="112"/>
+      <c r="AB32" s="112"/>
+      <c r="AC32" s="112"/>
+      <c r="AD32" s="112"/>
+      <c r="AE32" s="112"/>
+      <c r="AF32" s="112"/>
+      <c r="AG32" s="112"/>
+      <c r="AH32" s="112"/>
+      <c r="AI32" s="112"/>
+      <c r="AJ32" s="113"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="15">
+    <mergeCell ref="C29:AJ30"/>
+    <mergeCell ref="C31:AJ32"/>
+    <mergeCell ref="Z4:AC4"/>
+    <mergeCell ref="AG4:AJ4"/>
+    <mergeCell ref="E23:AJ24"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="E1:V2"/>
     <mergeCell ref="W1:AJ1"/>
@@ -3400,11 +4215,6 @@
     <mergeCell ref="M3:V4"/>
     <mergeCell ref="Z3:AC3"/>
     <mergeCell ref="AG3:AJ3"/>
-    <mergeCell ref="C29:AJ30"/>
-    <mergeCell ref="C31:AJ32"/>
-    <mergeCell ref="Z4:AC4"/>
-    <mergeCell ref="AG4:AJ4"/>
-    <mergeCell ref="E23:AJ24"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.3" top="0.4" bottom="0.3" header="0.15" footer="0.15"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3417,140 +4227,140 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ8"/>
+  <dimension ref="A1:AJ29"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="81" t="s">
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="83"/>
-      <c r="W1" s="87" t="s">
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="80"/>
+      <c r="P1" s="80"/>
+      <c r="Q1" s="80"/>
+      <c r="R1" s="80"/>
+      <c r="S1" s="80"/>
+      <c r="T1" s="80"/>
+      <c r="U1" s="80"/>
+      <c r="V1" s="81"/>
+      <c r="W1" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="88"/>
-      <c r="Y1" s="88"/>
-      <c r="Z1" s="88"/>
-      <c r="AA1" s="88"/>
-      <c r="AB1" s="88"/>
-      <c r="AC1" s="88"/>
-      <c r="AD1" s="88"/>
-      <c r="AE1" s="88"/>
-      <c r="AF1" s="88"/>
-      <c r="AG1" s="88"/>
-      <c r="AH1" s="88"/>
-      <c r="AI1" s="88"/>
-      <c r="AJ1" s="89"/>
+      <c r="X1" s="86"/>
+      <c r="Y1" s="86"/>
+      <c r="Z1" s="86"/>
+      <c r="AA1" s="86"/>
+      <c r="AB1" s="86"/>
+      <c r="AC1" s="86"/>
+      <c r="AD1" s="86"/>
+      <c r="AE1" s="86"/>
+      <c r="AF1" s="86"/>
+      <c r="AG1" s="86"/>
+      <c r="AH1" s="86"/>
+      <c r="AI1" s="86"/>
+      <c r="AJ1" s="87"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="79"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
-      <c r="R2" s="85"/>
-      <c r="S2" s="85"/>
-      <c r="T2" s="85"/>
-      <c r="U2" s="85"/>
-      <c r="V2" s="86"/>
-      <c r="W2" s="90" t="s">
+      <c r="A2" s="77"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
+      <c r="S2" s="83"/>
+      <c r="T2" s="83"/>
+      <c r="U2" s="83"/>
+      <c r="V2" s="84"/>
+      <c r="W2" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="X2" s="91"/>
-      <c r="Y2" s="91"/>
-      <c r="Z2" s="91"/>
-      <c r="AA2" s="91"/>
-      <c r="AB2" s="91"/>
-      <c r="AC2" s="91"/>
-      <c r="AD2" s="91"/>
-      <c r="AE2" s="91"/>
-      <c r="AF2" s="91"/>
-      <c r="AG2" s="91"/>
-      <c r="AH2" s="91"/>
-      <c r="AI2" s="91"/>
-      <c r="AJ2" s="92"/>
+      <c r="X2" s="89"/>
+      <c r="Y2" s="89"/>
+      <c r="Z2" s="89"/>
+      <c r="AA2" s="89"/>
+      <c r="AB2" s="89"/>
+      <c r="AC2" s="89"/>
+      <c r="AD2" s="89"/>
+      <c r="AE2" s="89"/>
+      <c r="AF2" s="89"/>
+      <c r="AG2" s="89"/>
+      <c r="AH2" s="89"/>
+      <c r="AI2" s="89"/>
+      <c r="AJ2" s="90"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="94"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="97" t="s">
+      <c r="B3" s="92"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="95" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="94" t="s">
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="94"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="103"/>
-      <c r="M3" s="105" t="s">
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
-      <c r="Q3" s="98"/>
-      <c r="R3" s="98"/>
-      <c r="S3" s="98"/>
-      <c r="T3" s="98"/>
-      <c r="U3" s="98"/>
-      <c r="V3" s="106"/>
+      <c r="N3" s="96"/>
+      <c r="O3" s="96"/>
+      <c r="P3" s="96"/>
+      <c r="Q3" s="96"/>
+      <c r="R3" s="96"/>
+      <c r="S3" s="96"/>
+      <c r="T3" s="96"/>
+      <c r="U3" s="96"/>
+      <c r="V3" s="104"/>
       <c r="W3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
-      <c r="Z3" s="72">
+      <c r="Z3" s="107">
         <v>43224</v>
       </c>
-      <c r="AA3" s="72"/>
-      <c r="AB3" s="72"/>
-      <c r="AC3" s="73"/>
+      <c r="AA3" s="107"/>
+      <c r="AB3" s="107"/>
+      <c r="AC3" s="108"/>
       <c r="AD3" s="3" t="s">
         <v>9</v>
       </c>
@@ -3562,46 +4372,46 @@
       <c r="AJ3" s="111"/>
     </row>
     <row r="4" spans="1:36" ht="15" customHeight="1">
-      <c r="A4" s="95"/>
-      <c r="B4" s="96"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="104"/>
-      <c r="M4" s="107"/>
-      <c r="N4" s="101"/>
-      <c r="O4" s="101"/>
-      <c r="P4" s="101"/>
-      <c r="Q4" s="101"/>
-      <c r="R4" s="101"/>
-      <c r="S4" s="101"/>
-      <c r="T4" s="101"/>
-      <c r="U4" s="101"/>
-      <c r="V4" s="108"/>
+      <c r="A4" s="93"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="94"/>
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
+      <c r="L4" s="102"/>
+      <c r="M4" s="105"/>
+      <c r="N4" s="99"/>
+      <c r="O4" s="99"/>
+      <c r="P4" s="99"/>
+      <c r="Q4" s="99"/>
+      <c r="R4" s="99"/>
+      <c r="S4" s="99"/>
+      <c r="T4" s="99"/>
+      <c r="U4" s="99"/>
+      <c r="V4" s="106"/>
       <c r="W4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
-      <c r="Z4" s="72"/>
-      <c r="AA4" s="72"/>
-      <c r="AB4" s="72"/>
-      <c r="AC4" s="73"/>
+      <c r="Z4" s="107"/>
+      <c r="AA4" s="107"/>
+      <c r="AB4" s="107"/>
+      <c r="AC4" s="108"/>
       <c r="AD4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AE4" s="7"/>
       <c r="AF4" s="8"/>
-      <c r="AG4" s="74"/>
-      <c r="AH4" s="75"/>
-      <c r="AI4" s="75"/>
-      <c r="AJ4" s="76"/>
+      <c r="AG4" s="114"/>
+      <c r="AH4" s="115"/>
+      <c r="AI4" s="115"/>
+      <c r="AJ4" s="116"/>
     </row>
     <row r="5" spans="1:36" ht="15.75">
       <c r="A5" s="35">
@@ -3686,48 +4496,103 @@
       <c r="AJ6" s="42"/>
     </row>
     <row r="7" spans="1:36" ht="15.75">
-      <c r="A7" s="114"/>
-      <c r="B7" s="115" t="s">
+      <c r="A7" s="70"/>
+      <c r="B7" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="117"/>
-      <c r="D7" s="117"/>
-      <c r="E7" s="117"/>
-      <c r="F7" s="117"/>
-      <c r="G7" s="117"/>
-      <c r="H7" s="117"/>
-      <c r="I7" s="117"/>
-      <c r="J7" s="117"/>
-      <c r="K7" s="117"/>
-      <c r="L7" s="117"/>
-      <c r="M7" s="117"/>
-      <c r="N7" s="117"/>
-      <c r="O7" s="117"/>
-      <c r="P7" s="117"/>
-      <c r="Q7" s="117"/>
-      <c r="R7" s="117"/>
-      <c r="S7" s="117"/>
-      <c r="T7" s="117"/>
-      <c r="U7" s="117"/>
-      <c r="V7" s="117"/>
-      <c r="W7" s="117"/>
-      <c r="X7" s="117"/>
-      <c r="Y7" s="117"/>
-      <c r="Z7" s="117"/>
-      <c r="AA7" s="117"/>
-      <c r="AB7" s="117"/>
-      <c r="AC7" s="117"/>
-      <c r="AD7" s="117"/>
-      <c r="AE7" s="117"/>
-      <c r="AF7" s="117"/>
-      <c r="AG7" s="117"/>
-      <c r="AH7" s="117"/>
-      <c r="AI7" s="117"/>
-      <c r="AJ7" s="118"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="73"/>
+      <c r="R7" s="73"/>
+      <c r="S7" s="73"/>
+      <c r="T7" s="73"/>
+      <c r="U7" s="73"/>
+      <c r="V7" s="73"/>
+      <c r="W7" s="73"/>
+      <c r="X7" s="73"/>
+      <c r="Y7" s="73"/>
+      <c r="Z7" s="73"/>
+      <c r="AA7" s="73"/>
+      <c r="AB7" s="73"/>
+      <c r="AC7" s="73"/>
+      <c r="AD7" s="73"/>
+      <c r="AE7" s="73"/>
+      <c r="AF7" s="73"/>
+      <c r="AG7" s="73"/>
+      <c r="AH7" s="73"/>
+      <c r="AI7" s="73"/>
+      <c r="AJ7" s="74"/>
     </row>
     <row r="8" spans="1:36">
-      <c r="A8" s="116"/>
-      <c r="B8" s="116"/>
+      <c r="A8" s="72"/>
+      <c r="B8" s="119"/>
+      <c r="C8" s="120"/>
+      <c r="D8" s="120"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="120"/>
+      <c r="G8" s="120"/>
+      <c r="H8" s="120"/>
+      <c r="I8" s="120"/>
+      <c r="J8" s="120"/>
+      <c r="K8" s="121" t="s">
+        <v>51</v>
+      </c>
+      <c r="L8" s="122"/>
+      <c r="M8" s="122" t="s">
+        <v>50</v>
+      </c>
+      <c r="N8" s="122"/>
+      <c r="O8" s="122"/>
+      <c r="P8" s="122"/>
+      <c r="Q8" s="122"/>
+      <c r="R8" s="122"/>
+      <c r="S8" s="122"/>
+      <c r="T8" s="122"/>
+      <c r="U8" s="122"/>
+      <c r="V8" s="122"/>
+      <c r="W8" s="122"/>
+      <c r="X8" s="122"/>
+      <c r="Y8" s="122"/>
+      <c r="Z8" s="122"/>
+      <c r="AA8" s="122"/>
+      <c r="AB8" s="122"/>
+      <c r="AC8" s="122"/>
+      <c r="AD8" s="122"/>
+      <c r="AE8" s="122"/>
+      <c r="AF8" s="122"/>
+      <c r="AG8" s="122"/>
+    </row>
+    <row r="26" spans="13:13">
+      <c r="M26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="13:13">
+      <c r="M27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="13:13">
+      <c r="M28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="13:13">
+      <c r="M29" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -3751,5 +4616,6 @@
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>